<commit_message>
Add Use case descriptions
</commit_message>
<xml_diff>
--- a/gantt-chart_L.xlsx
+++ b/gantt-chart_L.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTCS5607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063E8AE-3BCC-43E9-93BD-A146726C608B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8555B68E-06F5-4F8C-B8EF-2E6E2E77F55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1746,12 +1746,6 @@
     <t>Software Configuration</t>
   </si>
   <si>
-    <t>Preparation for Presentation</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
     <t>User Training</t>
   </si>
   <si>
@@ -1813,6 +1807,12 @@
   </si>
   <si>
     <t>1.8.1</t>
+  </si>
+  <si>
+    <t>Database Testing</t>
+  </si>
+  <si>
+    <t>Launch</t>
   </si>
 </sst>
 </file>
@@ -3198,6 +3198,13 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3207,6 +3214,10 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="166" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3215,17 +3226,6 @@
     </xf>
     <xf numFmtId="166" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4074,7 +4074,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4102,29 +4102,29 @@
       <c r="E1" s="152"/>
       <c r="F1" s="152"/>
       <c r="I1" s="121"/>
-      <c r="K1" s="183" t="s">
+      <c r="K1" s="177" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="183"/>
-      <c r="R1" s="183"/>
-      <c r="S1" s="183"/>
-      <c r="T1" s="183"/>
-      <c r="U1" s="183"/>
-      <c r="V1" s="183"/>
-      <c r="W1" s="183"/>
-      <c r="X1" s="183"/>
-      <c r="Y1" s="183"/>
-      <c r="Z1" s="183"/>
-      <c r="AA1" s="183"/>
-      <c r="AB1" s="183"/>
-      <c r="AC1" s="183"/>
-      <c r="AD1" s="183"/>
-      <c r="AE1" s="183"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -4169,11 +4169,11 @@
       <c r="B4" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="185">
+      <c r="C4" s="182">
         <v>44459</v>
       </c>
-      <c r="D4" s="185"/>
-      <c r="E4" s="185"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
       <c r="F4" s="155"/>
       <c r="G4" s="105" t="s">
         <v>73</v>
@@ -4183,182 +4183,182 @@
       </c>
       <c r="I4" s="103"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="177" t="str">
+      <c r="K4" s="179" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="178"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="179"/>
-      <c r="R4" s="177" t="str">
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="180"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="179" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="178"/>
-      <c r="T4" s="178"/>
-      <c r="U4" s="178"/>
-      <c r="V4" s="178"/>
-      <c r="W4" s="178"/>
-      <c r="X4" s="179"/>
-      <c r="Y4" s="177" t="str">
+      <c r="S4" s="180"/>
+      <c r="T4" s="180"/>
+      <c r="U4" s="180"/>
+      <c r="V4" s="180"/>
+      <c r="W4" s="180"/>
+      <c r="X4" s="181"/>
+      <c r="Y4" s="179" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="178"/>
-      <c r="AA4" s="178"/>
-      <c r="AB4" s="178"/>
-      <c r="AC4" s="178"/>
-      <c r="AD4" s="178"/>
-      <c r="AE4" s="179"/>
-      <c r="AF4" s="177" t="str">
+      <c r="Z4" s="180"/>
+      <c r="AA4" s="180"/>
+      <c r="AB4" s="180"/>
+      <c r="AC4" s="180"/>
+      <c r="AD4" s="180"/>
+      <c r="AE4" s="181"/>
+      <c r="AF4" s="179" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="178"/>
-      <c r="AH4" s="178"/>
-      <c r="AI4" s="178"/>
-      <c r="AJ4" s="178"/>
-      <c r="AK4" s="178"/>
-      <c r="AL4" s="179"/>
-      <c r="AM4" s="177" t="str">
+      <c r="AG4" s="180"/>
+      <c r="AH4" s="180"/>
+      <c r="AI4" s="180"/>
+      <c r="AJ4" s="180"/>
+      <c r="AK4" s="180"/>
+      <c r="AL4" s="181"/>
+      <c r="AM4" s="179" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="178"/>
-      <c r="AO4" s="178"/>
-      <c r="AP4" s="178"/>
-      <c r="AQ4" s="178"/>
-      <c r="AR4" s="178"/>
-      <c r="AS4" s="179"/>
-      <c r="AT4" s="177" t="str">
+      <c r="AN4" s="180"/>
+      <c r="AO4" s="180"/>
+      <c r="AP4" s="180"/>
+      <c r="AQ4" s="180"/>
+      <c r="AR4" s="180"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="179" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="178"/>
-      <c r="AV4" s="178"/>
-      <c r="AW4" s="178"/>
-      <c r="AX4" s="178"/>
-      <c r="AY4" s="178"/>
-      <c r="AZ4" s="179"/>
-      <c r="BA4" s="177" t="str">
+      <c r="AU4" s="180"/>
+      <c r="AV4" s="180"/>
+      <c r="AW4" s="180"/>
+      <c r="AX4" s="180"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="181"/>
+      <c r="BA4" s="179" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="178"/>
-      <c r="BC4" s="178"/>
-      <c r="BD4" s="178"/>
-      <c r="BE4" s="178"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="179"/>
-      <c r="BH4" s="177" t="str">
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="180"/>
+      <c r="BG4" s="181"/>
+      <c r="BH4" s="179" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="178"/>
-      <c r="BJ4" s="178"/>
-      <c r="BK4" s="178"/>
-      <c r="BL4" s="178"/>
-      <c r="BM4" s="178"/>
-      <c r="BN4" s="179"/>
+      <c r="BI4" s="180"/>
+      <c r="BJ4" s="180"/>
+      <c r="BK4" s="180"/>
+      <c r="BL4" s="180"/>
+      <c r="BM4" s="180"/>
+      <c r="BN4" s="181"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="102"/>
       <c r="B5" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="184" t="s">
+      <c r="C5" s="178" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
       <c r="F5" s="156"/>
       <c r="G5" s="104"/>
       <c r="H5" s="104"/>
       <c r="I5" s="104"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="180">
+      <c r="K5" s="183">
         <f>K6</f>
         <v>44459</v>
       </c>
-      <c r="L5" s="181"/>
-      <c r="M5" s="181"/>
-      <c r="N5" s="181"/>
-      <c r="O5" s="181"/>
-      <c r="P5" s="181"/>
-      <c r="Q5" s="182"/>
-      <c r="R5" s="180">
+      <c r="L5" s="184"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="185"/>
+      <c r="R5" s="183">
         <f>R6</f>
         <v>44466</v>
       </c>
-      <c r="S5" s="181"/>
-      <c r="T5" s="181"/>
-      <c r="U5" s="181"/>
-      <c r="V5" s="181"/>
-      <c r="W5" s="181"/>
-      <c r="X5" s="182"/>
-      <c r="Y5" s="180">
+      <c r="S5" s="184"/>
+      <c r="T5" s="184"/>
+      <c r="U5" s="184"/>
+      <c r="V5" s="184"/>
+      <c r="W5" s="184"/>
+      <c r="X5" s="185"/>
+      <c r="Y5" s="183">
         <f>Y6</f>
         <v>44473</v>
       </c>
-      <c r="Z5" s="181"/>
-      <c r="AA5" s="181"/>
-      <c r="AB5" s="181"/>
-      <c r="AC5" s="181"/>
-      <c r="AD5" s="181"/>
-      <c r="AE5" s="182"/>
-      <c r="AF5" s="180">
+      <c r="Z5" s="184"/>
+      <c r="AA5" s="184"/>
+      <c r="AB5" s="184"/>
+      <c r="AC5" s="184"/>
+      <c r="AD5" s="184"/>
+      <c r="AE5" s="185"/>
+      <c r="AF5" s="183">
         <f>AF6</f>
         <v>44480</v>
       </c>
-      <c r="AG5" s="181"/>
-      <c r="AH5" s="181"/>
-      <c r="AI5" s="181"/>
-      <c r="AJ5" s="181"/>
-      <c r="AK5" s="181"/>
-      <c r="AL5" s="182"/>
-      <c r="AM5" s="180">
+      <c r="AG5" s="184"/>
+      <c r="AH5" s="184"/>
+      <c r="AI5" s="184"/>
+      <c r="AJ5" s="184"/>
+      <c r="AK5" s="184"/>
+      <c r="AL5" s="185"/>
+      <c r="AM5" s="183">
         <f>AM6</f>
         <v>44487</v>
       </c>
-      <c r="AN5" s="181"/>
-      <c r="AO5" s="181"/>
-      <c r="AP5" s="181"/>
-      <c r="AQ5" s="181"/>
-      <c r="AR5" s="181"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="180">
+      <c r="AN5" s="184"/>
+      <c r="AO5" s="184"/>
+      <c r="AP5" s="184"/>
+      <c r="AQ5" s="184"/>
+      <c r="AR5" s="184"/>
+      <c r="AS5" s="185"/>
+      <c r="AT5" s="183">
         <f>AT6</f>
         <v>44494</v>
       </c>
-      <c r="AU5" s="181"/>
-      <c r="AV5" s="181"/>
-      <c r="AW5" s="181"/>
-      <c r="AX5" s="181"/>
-      <c r="AY5" s="181"/>
-      <c r="AZ5" s="182"/>
-      <c r="BA5" s="180">
+      <c r="AU5" s="184"/>
+      <c r="AV5" s="184"/>
+      <c r="AW5" s="184"/>
+      <c r="AX5" s="184"/>
+      <c r="AY5" s="184"/>
+      <c r="AZ5" s="185"/>
+      <c r="BA5" s="183">
         <f>BA6</f>
         <v>44501</v>
       </c>
-      <c r="BB5" s="181"/>
-      <c r="BC5" s="181"/>
-      <c r="BD5" s="181"/>
-      <c r="BE5" s="181"/>
-      <c r="BF5" s="181"/>
-      <c r="BG5" s="182"/>
-      <c r="BH5" s="180">
+      <c r="BB5" s="184"/>
+      <c r="BC5" s="184"/>
+      <c r="BD5" s="184"/>
+      <c r="BE5" s="184"/>
+      <c r="BF5" s="184"/>
+      <c r="BG5" s="185"/>
+      <c r="BH5" s="183">
         <f>BH6</f>
         <v>44508</v>
       </c>
-      <c r="BI5" s="181"/>
-      <c r="BJ5" s="181"/>
-      <c r="BK5" s="181"/>
-      <c r="BL5" s="181"/>
-      <c r="BM5" s="181"/>
-      <c r="BN5" s="182"/>
+      <c r="BI5" s="184"/>
+      <c r="BJ5" s="184"/>
+      <c r="BK5" s="184"/>
+      <c r="BL5" s="184"/>
+      <c r="BM5" s="184"/>
+      <c r="BN5" s="185"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -5205,7 +5205,7 @@
         <v>44461</v>
       </c>
       <c r="F12" s="162">
-        <f t="shared" ref="F12:F20" si="7">IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+        <f t="shared" ref="F12:F19" si="7">IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
         <v>44461</v>
       </c>
       <c r="G12" s="61">
@@ -5954,7 +5954,7 @@
         <v>1.5</v>
       </c>
       <c r="B21" s="115" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C21" s="60" t="s">
         <v>136</v>
@@ -6296,7 +6296,7 @@
     </row>
     <row r="25" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="59" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B25" s="117" t="s">
         <v>146</v>
@@ -8150,10 +8150,10 @@
     </row>
     <row r="47" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="59" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B47" s="117" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C47" s="60" t="s">
         <v>136</v>
@@ -8234,10 +8234,10 @@
     </row>
     <row r="48" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C48" s="60" t="s">
         <v>136</v>
@@ -8318,10 +8318,10 @@
     </row>
     <row r="49" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="59" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B49" s="117" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C49" s="60" t="s">
         <v>136</v>
@@ -8405,7 +8405,7 @@
         <v>2.5</v>
       </c>
       <c r="B50" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C50" s="60" t="s">
         <v>136</v>
@@ -8486,7 +8486,7 @@
     </row>
     <row r="51" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="59" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B51" s="117" t="s">
         <v>155</v>
@@ -8567,7 +8567,7 @@
     </row>
     <row r="52" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="59" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B52" s="117" t="s">
         <v>154</v>
@@ -8648,7 +8648,7 @@
     </row>
     <row r="53" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B53" s="117" t="s">
         <v>156</v>
@@ -8729,7 +8729,7 @@
     </row>
     <row r="54" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="59" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B54" s="117" t="s">
         <v>158</v>
@@ -8810,7 +8810,7 @@
     </row>
     <row r="55" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="59" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B55" s="117" t="s">
         <v>160</v>
@@ -8891,7 +8891,7 @@
     </row>
     <row r="56" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="59" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B56" s="117" t="s">
         <v>163</v>
@@ -8972,7 +8972,7 @@
     </row>
     <row r="57" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B57" s="117" t="s">
         <v>164</v>
@@ -9053,7 +9053,7 @@
     </row>
     <row r="58" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="59" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B58" s="117" t="s">
         <v>166</v>
@@ -10991,7 +10991,7 @@
         <v>44504</v>
       </c>
       <c r="F81" s="162">
-        <f t="shared" ref="F81" si="9">IF(ISBLANK(E81)," - ",IF(G81=0,E81,E81+G81-1))</f>
+        <f t="shared" ref="F81:F82" si="9">IF(ISBLANK(E81)," - ",IF(G81=0,E81,E81+G81-1))</f>
         <v>44504</v>
       </c>
       <c r="G81" s="61">
@@ -11060,13 +11060,12 @@
       <c r="BM81" s="99"/>
       <c r="BN81" s="99"/>
     </row>
-    <row r="82" spans="1:66" s="60" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+    <row r="82" spans="1:66" s="60" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="59">
         <v>4.2</v>
       </c>
-      <c r="B82" s="115" t="s">
-        <v>208</v>
+      <c r="B82" s="176" t="s">
+        <v>232</v>
       </c>
       <c r="C82" s="60" t="s">
         <v>136</v>
@@ -11076,16 +11075,17 @@
         <v>44505</v>
       </c>
       <c r="F82" s="162">
-        <f t="shared" ref="F82" si="10">IF(ISBLANK(E82)," - ",IF(G82=0,E82,E82+G82-1))</f>
-        <v>44507</v>
+        <f t="shared" si="9"/>
+        <v>44505</v>
       </c>
       <c r="G82" s="61">
-        <v>3</v>
-      </c>
-      <c r="H82" s="62">
-        <v>0</v>
-      </c>
-      <c r="I82" s="63"/>
+        <v>1</v>
+      </c>
+      <c r="H82" s="62"/>
+      <c r="I82" s="63">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="J82" s="93"/>
       <c r="K82" s="99"/>
       <c r="L82" s="99"/>
@@ -11144,24 +11144,24 @@
       <c r="BM82" s="99"/>
       <c r="BN82" s="99"/>
     </row>
-    <row r="83" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:66" s="60" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B83" s="115" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C83" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D83" s="116"/>
       <c r="E83" s="161">
-        <v>44508</v>
+        <v>44505</v>
       </c>
       <c r="F83" s="162">
-        <f t="shared" si="6"/>
-        <v>44510</v>
+        <f t="shared" ref="F83" si="10">IF(ISBLANK(E83)," - ",IF(G83=0,E83,E83+G83-1))</f>
+        <v>44507</v>
       </c>
       <c r="G83" s="61">
         <v>3</v>
@@ -11169,10 +11169,7 @@
       <c r="H83" s="62">
         <v>0</v>
       </c>
-      <c r="I83" s="63">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
+      <c r="I83" s="63"/>
       <c r="J83" s="93"/>
       <c r="K83" s="99"/>
       <c r="L83" s="99"/>
@@ -11237,18 +11234,18 @@
         <v>4.4</v>
       </c>
       <c r="B84" s="115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C84" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="161">
-        <v>44511</v>
+        <v>44508</v>
       </c>
       <c r="F84" s="162">
         <f t="shared" si="6"/>
-        <v>44513</v>
+        <v>44510</v>
       </c>
       <c r="G84" s="61">
         <v>3</v>
@@ -11258,7 +11255,7 @@
       </c>
       <c r="I84" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J84" s="93"/>
       <c r="K84" s="99"/>
@@ -11324,28 +11321,28 @@
         <v>4.5</v>
       </c>
       <c r="B85" s="115" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C85" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D85" s="116"/>
       <c r="E85" s="161">
-        <v>44514</v>
+        <v>44511</v>
       </c>
       <c r="F85" s="162">
         <f t="shared" si="6"/>
-        <v>44517</v>
+        <v>44513</v>
       </c>
       <c r="G85" s="61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H85" s="62">
         <v>0</v>
       </c>
       <c r="I85" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J85" s="93"/>
       <c r="K85" s="99"/>
@@ -11410,12 +11407,12 @@
         <v>5</v>
       </c>
       <c r="B86" s="53" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="D86" s="55"/>
       <c r="E86" s="163"/>
       <c r="F86" s="163" t="str">
-        <f t="shared" ref="F86:F89" si="11">IF(ISBLANK(E86)," - ",IF(G86=0,E86,E86+G86-1))</f>
+        <f t="shared" ref="F86:F90" si="11">IF(ISBLANK(E86)," - ",IF(G86=0,E86,E86+G86-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G86" s="56"/>
@@ -11488,18 +11485,18 @@
         <v>5.1</v>
       </c>
       <c r="B87" s="115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C87" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D87" s="116"/>
       <c r="E87" s="161">
-        <v>44518</v>
+        <v>44514</v>
       </c>
       <c r="F87" s="162">
         <f t="shared" si="11"/>
-        <v>44519</v>
+        <v>44515</v>
       </c>
       <c r="G87" s="61">
         <v>2</v>
@@ -11509,7 +11506,7 @@
       </c>
       <c r="I87" s="63">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J87" s="93"/>
       <c r="K87" s="99"/>
@@ -11575,18 +11572,18 @@
         <v>5.2</v>
       </c>
       <c r="B88" s="115" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C88" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D88" s="116"/>
       <c r="E88" s="161">
-        <v>44520</v>
+        <v>44516</v>
       </c>
       <c r="F88" s="162">
         <f t="shared" si="11"/>
-        <v>44521</v>
+        <v>44517</v>
       </c>
       <c r="G88" s="61">
         <v>2</v>
@@ -11596,7 +11593,7 @@
       </c>
       <c r="I88" s="63">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J88" s="93"/>
       <c r="K88" s="99"/>
@@ -11661,18 +11658,18 @@
         <v>5.3</v>
       </c>
       <c r="B89" s="115" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C89" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D89" s="169"/>
       <c r="E89" s="170">
-        <v>44522</v>
+        <v>44518</v>
       </c>
       <c r="F89" s="162">
         <f t="shared" si="11"/>
-        <v>44522</v>
+        <v>44518</v>
       </c>
       <c r="G89" s="172">
         <v>1</v>
@@ -11742,17 +11739,18 @@
         <v>5.4</v>
       </c>
       <c r="B90" s="115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C90" s="60" t="s">
         <v>136</v>
       </c>
       <c r="D90" s="169"/>
       <c r="E90" s="170">
-        <v>44523</v>
-      </c>
-      <c r="F90" s="171">
-        <v>44523</v>
+        <v>44519</v>
+      </c>
+      <c r="F90" s="162">
+        <f t="shared" si="11"/>
+        <v>44519</v>
       </c>
       <c r="G90" s="172">
         <v>1</v>
@@ -12622,15 +12620,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -12641,9 +12630,18 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H91:H100 H83:H85 H8:H80">
+  <conditionalFormatting sqref="H91:H100 H84:H85 H8:H80">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -12694,7 +12692,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
+  <conditionalFormatting sqref="H83">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -12708,7 +12706,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
+  <conditionalFormatting sqref="H81:H82">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -12732,7 +12730,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A94:B94 A96:B96 B95 E26 E69 E80 E94:H96 G26:H26 G69:H69 G80:H80 H46 G97:G100 H28 H37 H70 H72 H85 H83 H84" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A94:B94 A96:B96 B95 E26 E69 E80 E94:H96 G26:H26 G69:H69 G80:H80 H46 G97:G100 H28 H37 H70 H72 H84 H85" unlockedFormula="1"/>
     <ignoredError sqref="A80 A69 A26" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -12781,7 +12779,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H91:H100 H83:H85 H8:H80</xm:sqref>
+          <xm:sqref>H91:H100 H84:H85 H8:H80</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{81583CEC-7F5F-4E46-98E4-AC29FDBC59D0}">
@@ -12811,7 +12809,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H82</xm:sqref>
+          <xm:sqref>H83</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7442C97C-5EBD-4EE1-AFFB-9CBCA499BBD1}">
@@ -12826,7 +12824,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H81</xm:sqref>
+          <xm:sqref>H81:H82</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>